<commit_message>
Updated spreadsheet to include 725329
</commit_message>
<xml_diff>
--- a/projects/patchseq_metadata/DT_HM_TissueClearingTracking_.xlsx
+++ b/projects/patchseq_metadata/DT_HM_TissueClearingTracking_.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alleninstitute.sharepoint.com/sites/U19Thalamus/Shared Documents/Project 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C658866D-8FF8-4A15-B93F-5F15C36201F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4D82684-9690-42E3-BCDB-63543431F6D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43410" yWindow="2320" windowWidth="28800" windowHeight="15370" firstSheet="9" activeTab="9" xr2:uid="{B817978D-3067-4F92-92E2-03C675FB59C4}"/>
+    <workbookView xWindow="43410" yWindow="2320" windowWidth="28800" windowHeight="15370" firstSheet="9" activeTab="11" xr2:uid="{B817978D-3067-4F92-92E2-03C675FB59C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Dec 2022 - Feb 2023" sheetId="7" r:id="rId1"/>
@@ -3065,10 +3065,10 @@
     <t xml:space="preserve">No U19 brains: 704242 is Anna Lakunina's; 724180 (spinal cord) is Judith Baka's; 725328, 726132, 726133 are Polina Kosillo's; 699463, 709319, 709322, 677150, 695941, 716324, 718451 are Kanghoon Jung's </t>
   </si>
   <si>
-    <t>721316, 698260, 709352, 704283, 725529, 703250, 705779, 703551, 705778, 722843, 718454, 687543</t>
-  </si>
-  <si>
-    <t xml:space="preserve">698260, 709352, 704283 are Anna Lakunina's; 725529 is Polina Kosillo's; 703250, 705779, 703551, 705778, 722843, 718454, 687543 are Kanghoon Jung's  </t>
+    <t>721316, 698260, 709352, 704283, 725329, 703250, 705779, 703551, 705778, 722843, 718454, 687543</t>
+  </si>
+  <si>
+    <t xml:space="preserve">698260, 709352, 704283 are Anna Lakunina's; 725329 is Polina Kosillo's; 703250, 705779, 703551, 705778, 722843, 718454, 687543 are Kanghoon Jung's  </t>
   </si>
   <si>
     <t>710110, 719360, 724927, 725326</t>
@@ -8481,7 +8481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBB4853B-27A2-4E9F-BB82-F5DF79FAE41D}">
   <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
@@ -9483,9 +9483,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22D1B779-0634-4F04-A0D7-CD3D69AAEDB4}">
   <dimension ref="A1:I148"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I135" sqref="I135"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C76" sqref="C76:K84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -10561,7 +10561,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="72.599999999999994">
+    <row r="77" spans="1:4" ht="76.5">
       <c r="A77" s="24">
         <v>76</v>
       </c>
@@ -10603,7 +10603,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="72.599999999999994">
+    <row r="80" spans="1:4" ht="76.5">
       <c r="A80" s="15">
         <v>79</v>
       </c>
@@ -17645,7 +17645,7 @@
   <dimension ref="A1:Y57"/>
   <sheetViews>
     <sheetView topLeftCell="A46" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="B56" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
@@ -25303,8 +25303,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A208028-4DB6-45B2-9FEA-F8072189C83A}">
   <dimension ref="A1:Y42"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -28070,7 +28071,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{497F0441-48A5-4434-AA45-80F3DAF71F4E}">
   <dimension ref="A1:Y30"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
@@ -30081,7 +30082,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{688584EE-3C7B-477C-A935-F812C1E46B0B}">
   <dimension ref="A1:Y33"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
@@ -32251,7 +32252,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD07617E-10EB-47A5-BFD2-7F25716D436B}">
   <dimension ref="A1:Y37"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q37" sqref="Q37"/>
     </sheetView>
   </sheetViews>
@@ -34725,6 +34726,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="4c65472c-b9f9-4571-94ff-540c94a616f5" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a192c208-c66a-4877-8c3a-71c84d8b7446">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DA38A99A95E53E45BC77383D06E8D8B8" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="98d2841fbb8db0096988a5f9c3b5b4a5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a192c208-c66a-4877-8c3a-71c84d8b7446" xmlns:ns3="4c65472c-b9f9-4571-94ff-540c94a616f5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f932ff0d344a76a8052b259bce753435" ns2:_="" ns3:_="">
     <xsd:import namespace="a192c208-c66a-4877-8c3a-71c84d8b7446"/>
@@ -34973,7 +34985,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -34982,25 +34994,14 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="4c65472c-b9f9-4571-94ff-540c94a616f5" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a192c208-c66a-4877-8c3a-71c84d8b7446">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC457C14-FD43-492D-99CE-65BB98327F62}"/>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2535C58-DF1C-4CCB-A971-F52E0C04C274}"/>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C88080F-69D8-4689-BEE5-A1C072168C04}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC457C14-FD43-492D-99CE-65BB98327F62}"/>
 </file>
</xml_diff>